<commit_message>
Enhanced visualizations and improved model training
</commit_message>
<xml_diff>
--- a/dyes_DFT_B3LYP_eth_dataset.xlsx
+++ b/dyes_DFT_B3LYP_eth_dataset.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,32 +456,17 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Total_Energy_Hartree</t>
+          <t>Max_Absorption_nm</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>Solvation_Energy_eV</t>
+          <t>Max_f_osc</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>Surface_Area_A2</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Molecular_Volume_A3</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Max_Absorption_nm</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Max_f_osc</t>
+          <t>Max_Excitation_eV</t>
         </is>
       </c>
     </row>
@@ -501,22 +486,13 @@
         <v>20.7259</v>
       </c>
       <c r="E2" t="n">
-        <v>-2864.079893</v>
+        <v>554</v>
       </c>
       <c r="F2" t="n">
-        <v>-1.117</v>
+        <v>0.993439</v>
       </c>
       <c r="G2" t="n">
-        <v>593.9405819999999</v>
-      </c>
-      <c r="H2" t="n">
-        <v>650.812005</v>
-      </c>
-      <c r="I2" t="n">
-        <v>554</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0.993439</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="3">
@@ -535,22 +511,13 @@
         <v>14.1902</v>
       </c>
       <c r="E3" t="n">
-        <v>-2683.053369</v>
+        <v>517</v>
       </c>
       <c r="F3" t="n">
-        <v>-1.022</v>
+        <v>0.60955</v>
       </c>
       <c r="G3" t="n">
-        <v>764.918353</v>
-      </c>
-      <c r="H3" t="n">
-        <v>839.174714</v>
-      </c>
-      <c r="I3" t="n">
-        <v>517</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0.60955</v>
+        <v>2.4</v>
       </c>
     </row>
     <row r="4">
@@ -569,22 +536,13 @@
         <v>12.8122</v>
       </c>
       <c r="E4" t="n">
-        <v>-2528.120347</v>
+        <v>534</v>
       </c>
       <c r="F4" t="n">
-        <v>-0.977</v>
+        <v>0.550979</v>
       </c>
       <c r="G4" t="n">
-        <v>702.50724</v>
-      </c>
-      <c r="H4" t="n">
-        <v>768.572942</v>
-      </c>
-      <c r="I4" t="n">
-        <v>534</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0.550979</v>
+        <v>2.32</v>
       </c>
     </row>
     <row r="5">
@@ -603,22 +561,13 @@
         <v>17.9826</v>
       </c>
       <c r="E5" t="n">
-        <v>-2864.07897</v>
+        <v>544</v>
       </c>
       <c r="F5" t="n">
-        <v>-1.107</v>
+        <v>0.742578</v>
       </c>
       <c r="G5" t="n">
-        <v>595.478938</v>
-      </c>
-      <c r="H5" t="n">
-        <v>648.763049</v>
-      </c>
-      <c r="I5" t="n">
-        <v>544</v>
-      </c>
-      <c r="J5" t="n">
-        <v>0.742578</v>
+        <v>2.28</v>
       </c>
     </row>
     <row r="6">
@@ -637,22 +586,13 @@
         <v>12.661</v>
       </c>
       <c r="E6" t="n">
-        <v>-3507.55295</v>
+        <v>555</v>
       </c>
       <c r="F6" t="n">
-        <v>-0.913</v>
+        <v>0.832417</v>
       </c>
       <c r="G6" t="n">
-        <v>580.355407</v>
-      </c>
-      <c r="H6" t="n">
-        <v>634.169887</v>
-      </c>
-      <c r="I6" t="n">
-        <v>555</v>
-      </c>
-      <c r="J6" t="n">
-        <v>0.832417</v>
+        <v>2.24</v>
       </c>
     </row>
     <row r="7">
@@ -671,22 +611,13 @@
         <v>14.1606</v>
       </c>
       <c r="E7" t="n">
-        <v>-1989.414128</v>
+        <v>500</v>
       </c>
       <c r="F7" t="n">
-        <v>-0.92</v>
+        <v>1.031302</v>
       </c>
       <c r="G7" t="n">
-        <v>539.874024</v>
-      </c>
-      <c r="H7" t="n">
-        <v>576.1362779999999</v>
-      </c>
-      <c r="I7" t="n">
-        <v>500</v>
-      </c>
-      <c r="J7" t="n">
-        <v>1.031302</v>
+        <v>2.48</v>
       </c>
     </row>
     <row r="8">
@@ -705,22 +636,13 @@
         <v>18.8847</v>
       </c>
       <c r="E8" t="n">
-        <v>-2220.611022</v>
+        <v>536</v>
       </c>
       <c r="F8" t="n">
-        <v>-1.095</v>
+        <v>0.862689</v>
       </c>
       <c r="G8" t="n">
-        <v>610.868691</v>
-      </c>
-      <c r="H8" t="n">
-        <v>666.812287</v>
-      </c>
-      <c r="I8" t="n">
-        <v>536</v>
-      </c>
-      <c r="J8" t="n">
-        <v>0.862689</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="9">
@@ -739,22 +661,13 @@
         <v>17.2652</v>
       </c>
       <c r="E9" t="n">
-        <v>-2773.56467</v>
+        <v>577</v>
       </c>
       <c r="F9" t="n">
-        <v>-1.212</v>
+        <v>0.531098</v>
       </c>
       <c r="G9" t="n">
-        <v>674.391241</v>
-      </c>
-      <c r="H9" t="n">
-        <v>744.380638</v>
-      </c>
-      <c r="I9" t="n">
-        <v>577</v>
-      </c>
-      <c r="J9" t="n">
-        <v>0.531098</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="10">
@@ -773,22 +686,13 @@
         <v>13.7921</v>
       </c>
       <c r="E10" t="n">
-        <v>-3326.532883</v>
+        <v>660</v>
       </c>
       <c r="F10" t="n">
-        <v>-1.067</v>
+        <v>1.038181</v>
       </c>
       <c r="G10" t="n">
-        <v>749.3071179999999</v>
-      </c>
-      <c r="H10" t="n">
-        <v>828.871728</v>
-      </c>
-      <c r="I10" t="n">
-        <v>660</v>
-      </c>
-      <c r="J10" t="n">
-        <v>1.038181</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="11">
@@ -807,22 +711,13 @@
         <v>6.413</v>
       </c>
       <c r="E11" t="n">
-        <v>-1396.083522</v>
+        <v>399</v>
       </c>
       <c r="F11" t="n">
-        <v>-1.145</v>
+        <v>0.224655</v>
       </c>
       <c r="G11" t="n">
-        <v>386.278717</v>
-      </c>
-      <c r="H11" t="n">
-        <v>410.712528</v>
-      </c>
-      <c r="I11" t="n">
-        <v>399</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0.224655</v>
+        <v>3.11</v>
       </c>
     </row>
     <row r="12">
@@ -841,22 +736,13 @@
         <v>6.5263</v>
       </c>
       <c r="E12" t="n">
-        <v>-1281.352513</v>
+        <v>402</v>
       </c>
       <c r="F12" t="n">
-        <v>-1.003</v>
+        <v>0.227484</v>
       </c>
       <c r="G12" t="n">
-        <v>354.085821</v>
-      </c>
-      <c r="H12" t="n">
-        <v>379.731455</v>
-      </c>
-      <c r="I12" t="n">
-        <v>402</v>
-      </c>
-      <c r="J12" t="n">
-        <v>0.227484</v>
+        <v>3.08</v>
       </c>
     </row>
     <row r="13">
@@ -875,22 +761,13 @@
         <v>6.9715</v>
       </c>
       <c r="E13" t="n">
-        <v>-1447.944334</v>
+        <v>405</v>
       </c>
       <c r="F13" t="n">
-        <v>-1.233</v>
+        <v>0.152135</v>
       </c>
       <c r="G13" t="n">
-        <v>363.908642</v>
-      </c>
-      <c r="H13" t="n">
-        <v>409.194773</v>
-      </c>
-      <c r="I13" t="n">
-        <v>405</v>
-      </c>
-      <c r="J13" t="n">
-        <v>0.152135</v>
+        <v>3.06</v>
       </c>
     </row>
     <row r="14">
@@ -909,22 +786,13 @@
         <v>5.7525</v>
       </c>
       <c r="E14" t="n">
-        <v>-3701.409329</v>
+        <v>469</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.646</v>
+        <v>0.484837</v>
       </c>
       <c r="G14" t="n">
-        <v>389.941995</v>
-      </c>
-      <c r="H14" t="n">
-        <v>426.242466</v>
-      </c>
-      <c r="I14" t="n">
-        <v>469</v>
-      </c>
-      <c r="J14" t="n">
-        <v>0.484837</v>
+        <v>2.65</v>
       </c>
     </row>
     <row r="15">
@@ -943,22 +811,13 @@
         <v>7.8539</v>
       </c>
       <c r="E15" t="n">
-        <v>-3793.764807</v>
+        <v>510</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.789</v>
+        <v>0.541924</v>
       </c>
       <c r="G15" t="n">
-        <v>408.19568</v>
-      </c>
-      <c r="H15" t="n">
-        <v>448.500504</v>
-      </c>
-      <c r="I15" t="n">
-        <v>510</v>
-      </c>
-      <c r="J15" t="n">
-        <v>0.541924</v>
+        <v>2.43</v>
       </c>
     </row>
     <row r="16">
@@ -977,22 +836,13 @@
         <v>8.835699999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>-1354.517108</v>
+        <v>341</v>
       </c>
       <c r="F16" t="n">
-        <v>-0.733</v>
+        <v>0.281546</v>
       </c>
       <c r="G16" t="n">
-        <v>328.278335</v>
-      </c>
-      <c r="H16" t="n">
-        <v>347.801414</v>
-      </c>
-      <c r="I16" t="n">
-        <v>341</v>
-      </c>
-      <c r="J16" t="n">
-        <v>0.281546</v>
+        <v>3.64</v>
       </c>
     </row>
     <row r="17">
@@ -1011,22 +861,13 @@
         <v>7.0232</v>
       </c>
       <c r="E17" t="n">
-        <v>-1262.163458</v>
+        <v>305</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.596</v>
+        <v>0.300347</v>
       </c>
       <c r="G17" t="n">
-        <v>308.643467</v>
-      </c>
-      <c r="H17" t="n">
-        <v>324.387263</v>
-      </c>
-      <c r="I17" t="n">
-        <v>305</v>
-      </c>
-      <c r="J17" t="n">
-        <v>0.300347</v>
+        <v>4.06</v>
       </c>
     </row>
     <row r="18">
@@ -1045,22 +886,13 @@
         <v>8.6835</v>
       </c>
       <c r="E18" t="n">
-        <v>-955.323794</v>
+        <v>334</v>
       </c>
       <c r="F18" t="n">
-        <v>-0.743</v>
+        <v>0.335496</v>
       </c>
       <c r="G18" t="n">
-        <v>307.409667</v>
-      </c>
-      <c r="H18" t="n">
-        <v>323.412627</v>
-      </c>
-      <c r="I18" t="n">
-        <v>334</v>
-      </c>
-      <c r="J18" t="n">
-        <v>0.335496</v>
+        <v>3.71</v>
       </c>
     </row>
     <row r="19">
@@ -1079,22 +911,13 @@
         <v>8.583600000000001</v>
       </c>
       <c r="E19" t="n">
-        <v>-1033.947388</v>
+        <v>537</v>
       </c>
       <c r="F19" t="n">
-        <v>-0.732</v>
+        <v>0.447366</v>
       </c>
       <c r="G19" t="n">
-        <v>334.55414</v>
-      </c>
-      <c r="H19" t="n">
-        <v>359.200264</v>
-      </c>
-      <c r="I19" t="n">
-        <v>537</v>
-      </c>
-      <c r="J19" t="n">
-        <v>0.447366</v>
+        <v>2.31</v>
       </c>
     </row>
     <row r="20">
@@ -1113,22 +936,13 @@
         <v>13.5509</v>
       </c>
       <c r="E20" t="n">
-        <v>-1468.041293</v>
+        <v>527</v>
       </c>
       <c r="F20" t="n">
-        <v>-0.999</v>
+        <v>0.750572</v>
       </c>
       <c r="G20" t="n">
-        <v>374.598773</v>
-      </c>
-      <c r="H20" t="n">
-        <v>386.045833</v>
-      </c>
-      <c r="I20" t="n">
-        <v>527</v>
-      </c>
-      <c r="J20" t="n">
-        <v>0.750572</v>
+        <v>2.35</v>
       </c>
     </row>
     <row r="21">
@@ -1147,22 +961,13 @@
         <v>15.556</v>
       </c>
       <c r="E21" t="n">
-        <v>-1622.093882</v>
+        <v>480</v>
       </c>
       <c r="F21" t="n">
-        <v>-1.049</v>
+        <v>0.652343</v>
       </c>
       <c r="G21" t="n">
-        <v>416.471123</v>
-      </c>
-      <c r="H21" t="n">
-        <v>430.289706</v>
-      </c>
-      <c r="I21" t="n">
-        <v>480</v>
-      </c>
-      <c r="J21" t="n">
-        <v>0.652343</v>
+        <v>2.58</v>
       </c>
     </row>
     <row r="22">
@@ -1181,22 +986,13 @@
         <v>12.3411</v>
       </c>
       <c r="E22" t="n">
-        <v>-1637.063345</v>
+        <v>561</v>
       </c>
       <c r="F22" t="n">
-        <v>-0.961</v>
+        <v>0.84324</v>
       </c>
       <c r="G22" t="n">
-        <v>393.717989</v>
-      </c>
-      <c r="H22" t="n">
-        <v>414.802294</v>
-      </c>
-      <c r="I22" t="n">
-        <v>561</v>
-      </c>
-      <c r="J22" t="n">
-        <v>0.84324</v>
+        <v>2.21</v>
       </c>
     </row>
     <row r="23">
@@ -1215,22 +1011,13 @@
         <v>12.6625</v>
       </c>
       <c r="E23" t="n">
-        <v>-1791.119606</v>
+        <v>438</v>
       </c>
       <c r="F23" t="n">
-        <v>-1.015</v>
+        <v>0.529192</v>
       </c>
       <c r="G23" t="n">
-        <v>438.497325</v>
-      </c>
-      <c r="H23" t="n">
-        <v>457.193097</v>
-      </c>
-      <c r="I23" t="n">
-        <v>438</v>
-      </c>
-      <c r="J23" t="n">
-        <v>0.529192</v>
+        <v>2.83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>